<commit_message>
update accuracy table, still running logistic regression
</commit_message>
<xml_diff>
--- a/best_model_performance_v2.xlsx
+++ b/best_model_performance_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Northeastern courses\CS 5100\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adithyaabhishek/Desktop/FAI5100/NIH_Chest_XRays_Disease_Detection-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD284897-5CC7-4A55-B090-77A9AB282D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFF1B66-79B6-9A48-A601-B5F16AA7BE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9024DD29-FBB4-4EC1-9DE5-C3D906D15B79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{9024DD29-FBB4-4EC1-9DE5-C3D906D15B79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>Disease</t>
   </si>
@@ -123,6 +123,9 @@
   <si>
     <t>Extra Trees</t>
   </si>
+  <si>
+    <t>*</t>
+  </si>
 </sst>
 </file>
 
@@ -131,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +178,18 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -312,7 +327,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -333,14 +348,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,6 +370,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -679,51 +695,51 @@
       <selection sqref="A1:R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.33203125" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="7.6640625" customWidth="1"/>
-    <col min="14" max="14" width="7.44140625" customWidth="1"/>
-    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" customWidth="1"/>
+    <col min="14" max="14" width="7.5" customWidth="1"/>
+    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" customWidth="1"/>
     <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -737,7 +753,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
@@ -787,33 +803,33 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -860,7 +876,7 @@
         <v>0.52200000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
@@ -907,7 +923,7 @@
         <v>0.501</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -954,7 +970,7 @@
         <v>0.503</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
@@ -1001,7 +1017,7 @@
         <v>0.501</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
@@ -1048,7 +1064,7 @@
         <v>0.52800000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
@@ -1095,7 +1111,7 @@
         <v>0.52300000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1142,7 +1158,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
@@ -1189,7 +1205,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
@@ -1236,7 +1252,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1283,7 +1299,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
@@ -1330,7 +1346,7 @@
         <v>0.51700000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
@@ -1377,7 +1393,7 @@
         <v>0.50600000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
@@ -1424,7 +1440,7 @@
         <v>0.49299999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>18</v>
       </c>
@@ -1471,7 +1487,7 @@
         <v>0.54700000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -1902,37 +1918,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0181AB3-8BD6-4BC2-866A-03240A4B74BD}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:18" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-    </row>
-    <row r="2" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+    </row>
+    <row r="2" spans="1:18" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1952,7 +1968,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
         <v>23</v>
@@ -1982,11 +1998,11 @@
       <c r="K3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2022,7 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -2014,13 +2030,13 @@
         <v>0.56399999999999995</v>
       </c>
       <c r="C6" s="9">
-        <v>0.53200000000000003</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="D6" s="9">
-        <v>0.52900000000000003</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="E6">
-        <v>0.70099999999999996</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="F6" s="9">
         <v>0.72</v>
@@ -2030,19 +2046,20 @@
         <v>0.496</v>
       </c>
       <c r="I6">
-        <v>0.47399999999999998</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="J6">
-        <v>0.50900000000000001</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="K6">
-        <v>0.51300000000000001</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="L6">
-        <v>0.45700000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="O6" s="18"/>
+    </row>
+    <row r="7" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
@@ -2050,35 +2067,36 @@
         <v>0.61899999999999999</v>
       </c>
       <c r="C7" s="9">
-        <v>0.58099999999999996</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="D7" s="9">
-        <v>0.54600000000000004</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="E7">
-        <v>0.72099999999999997</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="F7" s="9">
-        <v>0.89600000000000002</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7">
         <v>0.442</v>
       </c>
       <c r="I7">
-        <v>0.499</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="J7">
-        <v>0.50600000000000001</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="K7">
-        <v>0.55900000000000005</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="L7">
-        <v>0.56100000000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="O7" s="18"/>
+    </row>
+    <row r="8" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -2086,13 +2104,13 @@
         <v>0.59499999999999997</v>
       </c>
       <c r="C8" s="9">
-        <v>0.55500000000000005</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="D8" s="9">
-        <v>0.55500000000000005</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="E8">
-        <v>0.69799999999999995</v>
+        <v>0.79800000000000004</v>
       </c>
       <c r="F8" s="9">
         <v>0.80400000000000005</v>
@@ -2102,19 +2120,20 @@
         <v>0.50800000000000001</v>
       </c>
       <c r="I8">
-        <v>0.45700000000000002</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="J8">
-        <v>0.46700000000000003</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="K8">
-        <v>0.47599999999999998</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="L8">
-        <v>0.45300000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="O8" s="18"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
@@ -2122,35 +2141,35 @@
         <v>0.63400000000000001</v>
       </c>
       <c r="C9" s="9">
-        <v>0.59399999999999997</v>
+        <v>0.77900000000000003</v>
       </c>
       <c r="D9" s="9">
-        <v>0.57699999999999996</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="E9">
-        <v>0.73699999999999999</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="F9" s="9">
-        <v>0.878</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9">
         <v>0.54300000000000004</v>
       </c>
       <c r="I9">
-        <v>0.41499999999999998</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="J9">
-        <v>0.51</v>
+        <v>0.77</v>
       </c>
       <c r="K9">
-        <v>0.48399999999999999</v>
+        <v>0.72899999999999998</v>
       </c>
       <c r="L9">
-        <v>0.47599999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.80400000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
@@ -2158,35 +2177,35 @@
         <v>0.56200000000000006</v>
       </c>
       <c r="C10" s="9">
-        <v>0.54</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="D10" s="9">
-        <v>0.53</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="E10">
-        <v>0.70599999999999996</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="F10" s="9">
-        <v>0.68</v>
+        <v>0.75</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10">
         <v>0.44</v>
       </c>
       <c r="I10">
-        <v>0.46200000000000002</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="J10">
-        <v>0.48699999999999999</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="K10">
-        <v>0.48299999999999998</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="L10">
-        <v>0.46200000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.74299999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
@@ -2194,35 +2213,35 @@
         <v>0.63400000000000001</v>
       </c>
       <c r="C11" s="9">
-        <v>0.58499999999999996</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="D11" s="9">
-        <v>0.57299999999999995</v>
+        <v>0.69</v>
       </c>
       <c r="E11">
-        <v>0.72799999999999998</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="F11" s="9">
-        <v>0.88900000000000001</v>
+        <v>0.753</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11">
         <v>0.46899999999999997</v>
       </c>
       <c r="I11">
-        <v>0.54400000000000004</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="J11">
-        <v>0.60899999999999999</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="K11">
-        <v>0.501</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="L11">
-        <v>0.48899999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.68100000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
@@ -2230,35 +2249,35 @@
         <v>0.64300000000000002</v>
       </c>
       <c r="C12" s="9">
-        <v>0.58799999999999997</v>
+        <v>0.66</v>
       </c>
       <c r="D12" s="9">
-        <v>0.58599999999999997</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="E12">
-        <v>0.753</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="F12" s="9">
-        <v>0.93500000000000005</v>
+        <v>0.77</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12">
         <v>0.496</v>
       </c>
       <c r="I12">
-        <v>0.39900000000000002</v>
+        <v>0.65</v>
       </c>
       <c r="J12">
-        <v>0.441</v>
+        <v>0.66300000000000003</v>
       </c>
       <c r="K12">
-        <v>0.47799999999999998</v>
+        <v>0.54</v>
       </c>
       <c r="L12">
-        <v>0.47699999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.67600000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
@@ -2266,35 +2285,35 @@
         <v>0.86099999999999999</v>
       </c>
       <c r="C13" s="9">
-        <v>0.76500000000000001</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="D13" s="9">
-        <v>0.69599999999999995</v>
+        <v>0.78</v>
       </c>
       <c r="E13">
-        <v>0.98199999999999998</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="F13" s="9">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I13">
-        <v>6.9000000000000006E-2</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="J13">
-        <v>0.41599999999999998</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="K13">
-        <v>0.41299999999999998</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="L13">
-        <v>0.22900000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.75800000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
@@ -2302,13 +2321,13 @@
         <v>0.55100000000000005</v>
       </c>
       <c r="C14" s="9">
-        <v>0.52600000000000002</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="D14" s="9">
-        <v>0.52300000000000002</v>
+        <v>0.623</v>
       </c>
       <c r="E14">
-        <v>0.73099999999999998</v>
+        <v>0.79</v>
       </c>
       <c r="F14" s="9">
         <v>0.70399999999999996</v>
@@ -2318,19 +2337,19 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="I14">
-        <v>0.48899999999999999</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="J14">
-        <v>0.50800000000000001</v>
+        <v>0.629</v>
       </c>
       <c r="K14">
         <v>0.49399999999999999</v>
       </c>
       <c r="L14">
-        <v>0.55120000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
@@ -2338,13 +2357,13 @@
         <v>0.59</v>
       </c>
       <c r="C15" s="9">
-        <v>0.56599999999999995</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="D15" s="9">
-        <v>0.54600000000000004</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="E15">
-        <v>0.68200000000000005</v>
+        <v>0.753</v>
       </c>
       <c r="F15" s="9">
         <v>0.753</v>
@@ -2354,19 +2373,19 @@
         <v>0.51100000000000001</v>
       </c>
       <c r="I15">
-        <v>0.56899999999999995</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J15">
-        <v>0.58299999999999996</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="K15">
-        <v>0.49199999999999999</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="L15">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
@@ -2374,13 +2393,13 @@
         <v>0.58599999999999997</v>
       </c>
       <c r="C16" s="9">
-        <v>0.54700000000000004</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="D16" s="9">
-        <v>0.53800000000000003</v>
+        <v>0.57699999999999996</v>
       </c>
       <c r="E16">
-        <v>0.68799999999999994</v>
+        <v>0.752</v>
       </c>
       <c r="F16" s="9">
         <v>0.74099999999999999</v>
@@ -2390,19 +2409,19 @@
         <v>0.54600000000000004</v>
       </c>
       <c r="I16">
-        <v>0.53800000000000003</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="J16">
-        <v>0.53900000000000003</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="K16">
-        <v>0.45900000000000002</v>
+        <v>0.52700000000000002</v>
       </c>
       <c r="L16">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.56799999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
@@ -2410,13 +2429,13 @@
         <v>0.61699999999999999</v>
       </c>
       <c r="C17" s="9">
-        <v>0.56000000000000005</v>
+        <v>0.63</v>
       </c>
       <c r="D17" s="9">
-        <v>0.57099999999999995</v>
+        <v>0.629</v>
       </c>
       <c r="E17">
-        <v>0.70199999999999996</v>
+        <v>0.77300000000000002</v>
       </c>
       <c r="F17" s="9">
         <v>0.85899999999999999</v>
@@ -2426,19 +2445,19 @@
         <v>0.45500000000000002</v>
       </c>
       <c r="I17">
-        <v>0.52700000000000002</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="J17">
-        <v>0.49199999999999999</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="K17">
-        <v>0.48699999999999999</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="L17">
-        <v>0.45300000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
@@ -2446,13 +2465,13 @@
         <v>0.67100000000000004</v>
       </c>
       <c r="C18" s="9">
-        <v>0.58699999999999997</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="D18" s="9">
-        <v>0.58199999999999996</v>
+        <v>0.56540000000000001</v>
       </c>
       <c r="E18">
-        <v>0.78</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="F18" s="9">
         <v>0.88100000000000001</v>
@@ -2462,19 +2481,19 @@
         <v>0.51700000000000002</v>
       </c>
       <c r="I18">
-        <v>0.62</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="J18">
-        <v>0.624</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="K18">
-        <v>0.371</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="L18">
-        <v>0.58499999999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.67300000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>18</v>
       </c>
@@ -2482,13 +2501,13 @@
         <v>0.59</v>
       </c>
       <c r="C19" s="9">
-        <v>0.55900000000000005</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="D19" s="9">
-        <v>0.55000000000000004</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="E19">
-        <v>0.68600000000000005</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="F19" s="9">
         <v>0.81</v>
@@ -2498,19 +2517,19 @@
         <v>0.50800000000000001</v>
       </c>
       <c r="I19">
-        <v>0.49299999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="J19">
-        <v>0.40100000000000002</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="K19">
-        <v>0.44</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="L19">
-        <v>0.47399999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -2520,19 +2539,19 @@
       </c>
       <c r="C21" s="4">
         <f t="shared" ref="C21:H21" si="0">AVERAGE(C6:C19)</f>
-        <v>0.5774999999999999</v>
+        <v>0.66957142857142848</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="0"/>
-        <v>0.56442857142857139</v>
+        <v>0.66967142857142847</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>0.73535714285714282</v>
+        <v>0.81321428571428567</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" si="0"/>
-        <v>0.82499999999999996</v>
+        <v>0.79635714285714287</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4">
@@ -2540,20 +2559,28 @@
         <v>0.46171428571428574</v>
       </c>
       <c r="I21" s="4">
-        <f>AVERAGE(H6:H19)</f>
-        <v>0.46171428571428574</v>
+        <f>AVERAGE(I6:I19)</f>
+        <v>0.64685714285714291</v>
       </c>
       <c r="J21" s="4">
         <f>AVERAGE(I6:I19)</f>
-        <v>0.46821428571428575</v>
+        <v>0.64685714285714291</v>
       </c>
       <c r="K21" s="4">
-        <f>AVERAGE(J6:J19)</f>
-        <v>0.50657142857142845</v>
+        <f>AVERAGE(K6:K19)</f>
+        <v>0.59992857142857137</v>
       </c>
       <c r="L21" s="4">
-        <f>AVERAGE(K6:K19)</f>
-        <v>0.47499999999999998</v>
+        <f>AVERAGE(L6:L19)</f>
+        <v>0.68685714285714283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2562,6 +2589,7 @@
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G4:L4"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="B6:G6 E7:G19">
     <cfRule type="colorScale" priority="29">
       <colorScale>

</xml_diff>